<commit_message>
Update comparison results - 2026-01-09 10:57:02
</commit_message>
<xml_diff>
--- a/Batch 5 - 09 Jan-Vivek.xlsx
+++ b/Batch 5 - 09 Jan-Vivek.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N151"/>
+  <dimension ref="A1:O151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +530,11 @@
           <t>Prompt</t>
         </is>
       </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>AI_Output</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">

</xml_diff>